<commit_message>
Other. Added pages for the customer and order application; created a common base.html template; added forms for order and customer using ListView and CreateView.
</commit_message>
<xml_diff>
--- a/robots.xlsx
+++ b/robots.xlsx
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,21 +566,6 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>X5</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>D2</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>